<commit_message>
Guitar Pedal 1590b Rev 3
Drastically cleaned up the PCB layout for the 1590B guitar pedal.  Updated it to be a 4 Layer board and replaced all SMD parts with through-hole parts.  Much easier to build now!
</commit_message>
<xml_diff>
--- a/GuitarPedal1590b/docs/Bill_of_Materials_BOM.xlsx
+++ b/GuitarPedal1590b/docs/Bill_of_Materials_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshep/Dev/DaisySeedProjects/GuitarPedal1590b/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CD3A23-F994-174E-9A9D-014B2BC155DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE74E61C-7871-8248-9F74-DCCFBD4B07EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48320" yWindow="660" windowWidth="25700" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38660" yWindow="960" windowWidth="25700" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="114">
   <si>
     <t>Item #</t>
   </si>
@@ -126,9 +126,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>SMD</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>Daisy Seed</t>
   </si>
   <si>
-    <t>Either Solder to Board directly using header pins, or use two 20pin female headers to make it removable.</t>
-  </si>
-  <si>
     <t>20 Pin Headers</t>
   </si>
   <si>
@@ -222,9 +216,6 @@
     <t>Panel Mount</t>
   </si>
   <si>
-    <t>ASIN: B096XJWZJQ</t>
-  </si>
-  <si>
     <t>1/4" Jack Female 6.35mm Stereo Socket PCB Mount</t>
   </si>
   <si>
@@ -256,17 +247,6 @@
   </si>
   <si>
     <t>2.2uH Inductor Iron Core</t>
-  </si>
-  <si>
-    <t>6mm LED</t>
-  </si>
-  <si>
-    <t>Connect circuit board pads to LED with 22 AWG wire so that the led can be mounted on the enclosure. Any led should work, there is a 220R resiter limited the current from the 3.3v source.</t>
-  </si>
-  <si>
-    <t>Make sure to wire center pin negative to be compativle with most guitar pedal power supplies! Connect circuit board pads to foot switch leads with 22 AWG wire so the jack can be mounted on the enclosure
-Used this part:
-https://www.amazon.com/dp/B096XJWZJQ</t>
   </si>
   <si>
     <t>Connect circuit board pads to foot switch leads with 22 AWG wire so the footswitch can be mounted on the enclosure.
@@ -277,12 +257,6 @@
     <t>POT1, POT2, POT3, POT4</t>
   </si>
   <si>
-    <t>10k Potentiameter Linear Taper (Type B)</t>
-  </si>
-  <si>
-    <t>Connect circuit board pads to each POT with 22 AWG wire so that the POTs can be mounted on the enclosure.</t>
-  </si>
-  <si>
     <t>R1, R2, R4, R5, R7, R8, R9, R10, R13,  R14</t>
   </si>
   <si>
@@ -319,9 +293,6 @@
     <t>100 Ohm Resistor Metal Film 1/4W +/-1%</t>
   </si>
   <si>
-    <t>R15, R19, R20</t>
-  </si>
-  <si>
     <t>220 Ohm Resistor Metal Film 1/4W +/-1%</t>
   </si>
   <si>
@@ -343,56 +314,21 @@
     <t>470 Ohm Resistor Metal Film 1/4W +/-1%</t>
   </si>
   <si>
-    <t>SW1, SW2</t>
-  </si>
-  <si>
-    <t>HiLetgo</t>
-  </si>
-  <si>
-    <t>ASIN: B079JBF815</t>
-  </si>
-  <si>
-    <t>ON/ON SPDT 3 Terminal 2 Position Toggle Switch MTS102</t>
-  </si>
-  <si>
-    <t>Connect circuit board pads to each switch with 22 AWG wire so that the switches can be mounted on the enclosure.
-Used this part:
-https://www.amazon.com/dp/B079JBF815</t>
-  </si>
-  <si>
     <t>STMicorelectronics</t>
   </si>
   <si>
-    <t>LD1117DT50TR</t>
-  </si>
-  <si>
-    <t>LDO Voltage Regulator 5.0V 0.9A Positive</t>
-  </si>
-  <si>
-    <t>TO-252-3</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/511-LD1117DT50-TR</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
     <t>CUI Inc.</t>
   </si>
   <si>
-    <t>PDS1-S5-S5-M</t>
-  </si>
-  <si>
     <t>Isolated DC/DC Converter 1W 4.5-5.5Vin 5Vout 200mA unreg iso</t>
   </si>
   <si>
     <t>Custom Package</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/490-PDS1-S5-S5-M</t>
-  </si>
-  <si>
     <t>Microchip Technology</t>
   </si>
   <si>
@@ -411,21 +347,12 @@
     <t>Texas Instruments</t>
   </si>
   <si>
-    <t>OPA1652AID</t>
-  </si>
-  <si>
     <t xml:space="preserve">IC OpAmp 2-Circuit </t>
   </si>
   <si>
     <t>IC OpAmp 4-Circuit</t>
   </si>
   <si>
-    <t>SOIC-8</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/595-OPA1652AID</t>
-  </si>
-  <si>
     <t>H11L1</t>
   </si>
   <si>
@@ -448,13 +375,76 @@
   </si>
   <si>
     <t>Ceramic Capacitor 100nF</t>
+  </si>
+  <si>
+    <t>Use two 20pin female headers to make a socket for the Seed.  This is needed since some components fit under the seed.</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/992-CON-SOCJ-2155</t>
+  </si>
+  <si>
+    <t>Gravitech</t>
+  </si>
+  <si>
+    <t>CON-SOCJ-2155</t>
+  </si>
+  <si>
+    <t>PCB Mount</t>
+  </si>
+  <si>
+    <t>3mm LED</t>
+  </si>
+  <si>
+    <t>Connect circuit board pads to LED with 22 AWG wire so that the led can be mounted on the enclosure. Any led should work, there is a 1k resistor to limit the current from the 3.3v source. I used these nice LED holders to mount on the enclosure: https://www.amazon.com/dp/B083Q9QMN4</t>
+  </si>
+  <si>
+    <t>10k Potentiameter Linear Taper (Type B) Long Pins</t>
+  </si>
+  <si>
+    <t>L4931CZ50-AP</t>
+  </si>
+  <si>
+    <t>LDO Voltage Regulators 5.0V 0.25A Positive</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/511-L4931CZ50-AP</t>
+  </si>
+  <si>
+    <t>TO-92</t>
+  </si>
+  <si>
+    <t>PDS1-S5-S5-D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/490-PDS1-S5-S5-D</t>
+  </si>
+  <si>
+    <t>OPA2134PA</t>
+  </si>
+  <si>
+    <t>8-DIP</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/595-OPA2134PA</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R19, R20</t>
+  </si>
+  <si>
+    <t>1K Ohm Resistor Metal Film 1/4W +/-1%</t>
+  </si>
+  <si>
+    <t>I used pots with long leads from Tayda.  They worked great.  https://www.taydaelectronics.com/potentiometer-variable-resistors/rotary-potentiometer/linear/tayda-10k-ohm-linear-taper-potentiometer-spline-shaft-pcb-mount-rv16196.html  or you can connect circuit board pads to each POT wires for non-long lead pots.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -491,6 +481,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -548,7 +544,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -598,6 +594,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -905,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="E11" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -957,28 +956,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="45">
@@ -986,25 +985,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C3" s="2">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="30">
@@ -1012,28 +1011,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="C4" s="1">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>26</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="15">
@@ -1041,25 +1040,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" s="15"/>
     </row>
@@ -1068,25 +1067,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15">
@@ -1094,25 +1093,25 @@
         <v>5</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15">
@@ -1120,25 +1119,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="105">
@@ -1146,57 +1145,57 @@
         <v>7</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
       </c>
       <c r="D9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>38</v>
-      </c>
       <c r="G9" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="120">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="26" customHeight="1">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>42</v>
+      <c r="D10" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>56</v>
+        <v>12</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30">
@@ -1204,28 +1203,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30">
@@ -1233,28 +1232,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C12" s="2">
         <v>2</v>
       </c>
       <c r="D12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1">
@@ -1262,84 +1261,84 @@
         <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:9" ht="75">
+    <row r="14" spans="1:9" ht="105">
       <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2">
         <v>2</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="45">
+        <v>12</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="135">
       <c r="A15" s="2">
         <v>13</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C15" s="2">
         <v>4</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>59</v>
+        <v>18</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>60</v>
+        <v>12</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45">
@@ -1347,25 +1346,25 @@
         <v>14</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C16" s="2">
         <v>10</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15">
@@ -1373,25 +1372,25 @@
         <v>15</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C17" s="2">
         <v>2</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15">
@@ -1399,51 +1398,51 @@
         <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C18" s="2">
         <v>2</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>73</v>
+      <c r="B19" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="C19" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15">
@@ -1451,25 +1450,25 @@
         <v>18</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1477,25 +1476,25 @@
         <v>19</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C21" s="11">
         <v>1</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I21" s="11"/>
     </row>
@@ -1504,56 +1503,54 @@
         <v>20</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C22" s="11">
         <v>1</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" ht="90">
+    <row r="23" spans="1:9">
       <c r="A23" s="11">
         <v>21</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>81</v>
+      <c r="B23" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="C23" s="11">
         <v>2</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>84</v>
+        <v>18</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>85</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="I23" s="11"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="11">
@@ -1566,22 +1563,22 @@
         <v>1</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>10</v>
+        <v>72</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1589,28 +1586,28 @@
         <v>23</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="C25" s="11">
         <v>1</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>93</v>
+        <v>74</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>10</v>
+        <v>76</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1618,28 +1615,28 @@
         <v>24</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26" s="11">
         <v>1</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1647,28 +1644,28 @@
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C27" s="11">
         <v>1</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>103</v>
+        <v>82</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>10</v>
+        <v>83</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1676,28 +1673,28 @@
         <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28" s="11">
         <v>1</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1882,7 +1879,9 @@
     <hyperlink ref="I25" r:id="rId5" xr:uid="{CCEFA8AE-B5E5-B542-9A94-05C6EE0386BE}"/>
     <hyperlink ref="I26" r:id="rId6" xr:uid="{04AAC3D9-518F-DF43-8D9F-500C377B974E}"/>
     <hyperlink ref="I27" r:id="rId7" xr:uid="{10210211-C02A-6242-A06D-257B5BEDBBF9}"/>
-    <hyperlink ref="I28" r:id="rId8" xr:uid="{F25F2715-BF35-C14D-AAA9-AF45B9818986}"/>
+    <hyperlink ref="I10" r:id="rId8" xr:uid="{3A50486B-EFB8-3C42-A260-36061CEC7211}"/>
+    <hyperlink ref="D10" r:id="rId9" display="https://www.mouser.com/manufacturer/gravitech/" xr:uid="{3F61889C-263C-3546-B96A-848C4B005F30}"/>
+    <hyperlink ref="I28" r:id="rId10" xr:uid="{F25F2715-BF35-C14D-AAA9-AF45B9818986}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>

</xml_diff>